<commit_message>
updated the inflation data
</commit_message>
<xml_diff>
--- a/excel_files/inflation_data_excel.xlsx
+++ b/excel_files/inflation_data_excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91978\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91978\Desktop\inflation_prediction_project\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56960A56-CB59-4D92-9104-7BE31C3DCDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7312058-93E1-43FD-9785-A82CE979588B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inflation_data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="mm/yyyy"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -511,7 +514,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -559,7 +562,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -868,10 +871,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B376"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A376"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>

</xml_diff>